<commit_message>
Changes related to serial numbers Changes in secret file
</commit_message>
<xml_diff>
--- a/templates/Division To division Transfer.xlsx
+++ b/templates/Division To division Transfer.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603DF294-4FCD-45EB-A4B9-E2219DD1299B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79B6C9F-616A-4C42-AB1F-4D19B351EF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB441E9F-4FBE-410A-8F63-C9ADD7579EED}"/>
   </bookViews>
   <sheets>
     <sheet name="8172-LOT-New" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="74">
   <si>
     <t>Site</t>
   </si>
@@ -129,9 +127,6 @@
   </si>
   <si>
     <t>LOC100</t>
-  </si>
-  <si>
-    <t>Prova-12,Prova-13</t>
   </si>
   <si>
     <t>multidiv LOT (Lot track)</t>
@@ -263,6 +258,9 @@
   </si>
   <si>
     <t>Con1</t>
+  </si>
+  <si>
+    <t>Total Serials To Be Transferred</t>
   </si>
 </sst>
 </file>
@@ -642,7 +640,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,16 +710,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -748,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -756,16 +754,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -777,10 +775,10 @@
         <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>
@@ -792,7 +790,7 @@
         <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -800,16 +798,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" t="s">
-        <v>73</v>
-      </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -821,10 +819,10 @@
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
         <v>24</v>
@@ -836,7 +834,7 @@
         <v>135</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -844,16 +842,16 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -880,7 +878,7 @@
         <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -888,16 +886,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
@@ -909,7 +907,7 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3">
         <v>100</v>
@@ -924,7 +922,7 @@
         <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -932,16 +930,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -968,7 +966,7 @@
         <v>35</v>
       </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -976,16 +974,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
@@ -997,7 +995,7 @@
         <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" s="3">
         <v>100</v>
@@ -1012,7 +1010,7 @@
         <v>50</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1020,16 +1018,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
@@ -1056,7 +1054,7 @@
         <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1064,17 +1062,17 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
@@ -1085,10 +1083,10 @@
         <v>22</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
         <v>24</v>
@@ -1100,7 +1098,7 @@
         <v>70</v>
       </c>
       <c r="N10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1108,17 +1106,17 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
       <c r="F11" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1127,7 @@
         <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11" s="3">
         <v>100</v>
@@ -1144,7 +1142,7 @@
         <v>75</v>
       </c>
       <c r="N11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1152,16 +1150,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -1188,7 +1186,7 @@
         <v>85</v>
       </c>
       <c r="N12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1196,17 +1194,17 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
       <c r="F13" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1215,7 @@
         <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J13" s="3">
         <v>100</v>
@@ -1232,7 +1230,7 @@
         <v>100</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1240,17 +1238,17 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
       <c r="F14" t="s">
         <v>19</v>
       </c>
@@ -1261,10 +1259,10 @@
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -1276,7 +1274,7 @@
         <v>130</v>
       </c>
       <c r="N14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1284,16 +1282,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -1305,10 +1303,10 @@
         <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K15" t="s">
         <v>24</v>
@@ -1320,7 +1318,7 @@
         <v>135</v>
       </c>
       <c r="N15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1328,16 +1326,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1349,7 +1347,7 @@
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J16" s="3">
         <v>100</v>
@@ -1364,7 +1362,7 @@
         <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1372,16 +1370,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -1408,7 +1406,7 @@
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1416,16 +1414,16 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -1437,7 +1435,7 @@
         <v>22</v>
       </c>
       <c r="I18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J18" s="3">
         <v>100</v>
@@ -1452,7 +1450,7 @@
         <v>50</v>
       </c>
       <c r="N18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1460,16 +1458,16 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>37</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -1496,7 +1494,7 @@
         <v>60</v>
       </c>
       <c r="N19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1504,17 +1502,17 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
       <c r="F20" t="s">
         <v>19</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>22</v>
       </c>
       <c r="I20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J20" s="3">
         <v>100</v>
@@ -1540,7 +1538,7 @@
         <v>75</v>
       </c>
       <c r="N20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1548,16 +1546,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
         <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>40</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
@@ -1584,7 +1582,7 @@
         <v>85</v>
       </c>
       <c r="N21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1592,17 +1590,17 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
         <v>39</v>
       </c>
-      <c r="E22" t="s">
-        <v>40</v>
-      </c>
       <c r="F22" t="s">
         <v>19</v>
       </c>
@@ -1613,7 +1611,7 @@
         <v>22</v>
       </c>
       <c r="I22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J22" s="3">
         <v>100</v>
@@ -1628,7 +1626,7 @@
         <v>100</v>
       </c>
       <c r="N22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1638,35 +1636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC1DFEE-D629-4FDC-BD24-59986DBA090D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD96595-CC9B-43E8-9C0B-F6C67405A893}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45282ED-5D47-4C55-80D7-8A71C27B67B4}">
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1676,16 +1650,16 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
@@ -1697,10 +1671,10 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
@@ -1712,7 +1686,7 @@
         <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1720,16 +1694,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1741,10 +1715,10 @@
         <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -1756,7 +1730,7 @@
         <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1764,16 +1738,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -1785,10 +1759,10 @@
         <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>
@@ -1800,7 +1774,7 @@
         <v>40</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1808,16 +1782,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1829,10 +1803,10 @@
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" t="s">
         <v>24</v>
@@ -1844,7 +1818,7 @@
         <v>55</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1852,17 +1826,17 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
@@ -1873,10 +1847,10 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
         <v>24</v>
@@ -1888,7 +1862,7 @@
         <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1896,17 +1870,17 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
@@ -1917,10 +1891,10 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
         <v>24</v>
@@ -1932,7 +1906,7 @@
         <v>80</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1940,17 +1914,17 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
       <c r="F7" t="s">
         <v>19</v>
       </c>
@@ -1961,10 +1935,10 @@
         <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" t="s">
         <v>24</v>
@@ -1976,7 +1950,7 @@
         <v>90</v>
       </c>
       <c r="N7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1984,31 +1958,31 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>43</v>
-      </c>
       <c r="J8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
         <v>24</v>
@@ -2020,7 +1994,7 @@
         <v>115</v>
       </c>
       <c r="N8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2028,16 +2002,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
@@ -2049,10 +2023,10 @@
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9" t="s">
         <v>24</v>
@@ -2064,7 +2038,7 @@
         <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2072,16 +2046,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -2093,10 +2067,10 @@
         <v>22</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
         <v>24</v>
@@ -2108,7 +2082,7 @@
         <v>40</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2116,17 +2090,17 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
       <c r="F11" t="s">
         <v>19</v>
       </c>
@@ -2137,10 +2111,10 @@
         <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" t="s">
         <v>24</v>
@@ -2152,7 +2126,7 @@
         <v>65</v>
       </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2160,17 +2134,17 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
@@ -2181,10 +2155,10 @@
         <v>22</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" t="s">
         <v>24</v>
@@ -2196,7 +2170,7 @@
         <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2204,31 +2178,31 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
         <v>42</v>
       </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" t="s">
-        <v>43</v>
-      </c>
       <c r="J13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K13" t="s">
         <v>24</v>
@@ -2240,7 +2214,7 @@
         <v>115</v>
       </c>
       <c r="N13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2248,17 +2222,17 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
         <v>39</v>
       </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
       <c r="F14" t="s">
         <v>19</v>
       </c>
@@ -2269,10 +2243,10 @@
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -2284,7 +2258,7 @@
         <v>105</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2292,17 +2266,17 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
@@ -2313,10 +2287,10 @@
         <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K15" t="s">
         <v>24</v>
@@ -2328,7 +2302,7 @@
         <v>130</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2336,16 +2310,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -2357,10 +2331,10 @@
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" t="s">
         <v>24</v>
@@ -2372,7 +2346,7 @@
         <v>30</v>
       </c>
       <c r="N16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2380,16 +2354,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -2401,10 +2375,10 @@
         <v>22</v>
       </c>
       <c r="I17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" t="s">
         <v>24</v>
@@ -2416,7 +2390,7 @@
         <v>55</v>
       </c>
       <c r="N17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2424,17 +2398,17 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>37</v>
       </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
       <c r="F19" t="s">
         <v>19</v>
       </c>
@@ -2445,10 +2419,10 @@
         <v>22</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" t="s">
         <v>24</v>
@@ -2460,7 +2434,7 @@
         <v>80</v>
       </c>
       <c r="N19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -2468,17 +2442,17 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
       <c r="F20" t="s">
         <v>19</v>
       </c>
@@ -2489,10 +2463,10 @@
         <v>22</v>
       </c>
       <c r="I20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" t="s">
         <v>24</v>
@@ -2504,7 +2478,7 @@
         <v>105</v>
       </c>
       <c r="N20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2512,12 +2486,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452DA90E-1723-4B6B-96A7-A982916890FA}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2529,7 +2503,7 @@
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
@@ -2561,7 +2535,7 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="I1" t="s">
         <v>14</v>
@@ -2601,8 +2575,8 @@
       <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
-        <v>30</v>
+      <c r="H2">
+        <v>3</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -2628,7 +2602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327BB445-E756-4647-886B-5441E232C968}">
   <dimension ref="A1:P1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Project To Project Transfer Template changes for other transactions.
</commit_message>
<xml_diff>
--- a/templates/Division To division Transfer.xlsx
+++ b/templates/Division To division Transfer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4105B60-03E3-4382-A09A-5EBB291E9E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0D7573-2459-4D4F-BF8A-68E8791368C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BB441E9F-4FBE-410A-8F63-C9ADD7579EED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BB441E9F-4FBE-410A-8F63-C9ADD7579EED}"/>
   </bookViews>
   <sheets>
     <sheet name="8177-LOT-New" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="71">
   <si>
     <t>Site</t>
   </si>
@@ -218,13 +218,46 @@
   </si>
   <si>
     <t>Rec (Receiving Location-1)</t>
+  </si>
+  <si>
+    <t>multidiv no track</t>
+  </si>
+  <si>
+    <t>547TS</t>
+  </si>
+  <si>
+    <t>9RH2F</t>
+  </si>
+  <si>
+    <t>9TIOK</t>
+  </si>
+  <si>
+    <t>B1N29</t>
+  </si>
+  <si>
+    <t>Pro-101</t>
+  </si>
+  <si>
+    <t>Pro-102</t>
+  </si>
+  <si>
+    <t>777 (BC Site)</t>
+  </si>
+  <si>
+    <t>BFLS (OH-Backflush location)</t>
+  </si>
+  <si>
+    <t>Scrp (Scrap Location)</t>
+  </si>
+  <si>
+    <t>Pro-201</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +284,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -272,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -280,6 +319,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,17 +634,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC26E65-409C-493E-ABD4-A039BE3F1B14}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
@@ -617,7 +657,7 @@
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -666,13 +706,13 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -683,8 +723,8 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>53</v>
+      <c r="I2" t="s">
+        <v>36</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -693,30 +733,24 @@
         <v>21</v>
       </c>
       <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>60</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -727,8 +761,8 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
-        <v>36</v>
+      <c r="I3" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -737,30 +771,21 @@
         <v>21</v>
       </c>
       <c r="L3">
-        <v>75</v>
-      </c>
-      <c r="M3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -781,27 +806,21 @@
         <v>21</v>
       </c>
       <c r="L4">
-        <v>25</v>
-      </c>
-      <c r="M4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -822,30 +841,24 @@
         <v>21</v>
       </c>
       <c r="L5">
-        <v>35</v>
-      </c>
-      <c r="M5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
+        <v>66</v>
+      </c>
+      <c r="F6">
+        <v>1001</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -863,27 +876,21 @@
         <v>21</v>
       </c>
       <c r="L6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -904,27 +911,21 @@
         <v>21</v>
       </c>
       <c r="L7">
-        <v>85</v>
-      </c>
-      <c r="M7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -945,27 +946,21 @@
         <v>21</v>
       </c>
       <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -977,7 +972,7 @@
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -986,27 +981,21 @@
         <v>21</v>
       </c>
       <c r="L9">
-        <v>10</v>
-      </c>
-      <c r="M9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1018,7 +1007,7 @@
         <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
         <v>19</v>
@@ -1027,13 +1016,374 @@
         <v>21</v>
       </c>
       <c r="L10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11">
         <v>135</v>
       </c>
-      <c r="M10" t="s">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12">
+        <v>60</v>
+      </c>
+      <c r="M12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13">
+        <v>75</v>
+      </c>
+      <c r="M13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15">
+        <v>35</v>
+      </c>
+      <c r="M15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17">
+        <v>85</v>
+      </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18">
+        <v>10</v>
+      </c>
+      <c r="M18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19">
+        <v>135</v>
+      </c>
+      <c r="M19" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1041,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452DA90E-1723-4B6B-96A7-A982916890FA}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,16 +1464,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
+        <v>60</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -1135,10 +1482,10 @@
         <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>19</v>
@@ -1149,25 +1496,19 @@
       <c r="M2">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1179,10 +1520,10 @@
         <v>18</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>70</v>
       </c>
       <c r="K3" t="s">
         <v>19</v>
@@ -1191,24 +1532,21 @@
         <v>20</v>
       </c>
       <c r="M3">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
+      <c r="A4" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -1219,11 +1557,11 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="3">
-        <v>100</v>
+      <c r="I4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
       </c>
       <c r="K4" t="s">
         <v>19</v>
@@ -1232,10 +1570,7 @@
         <v>20</v>
       </c>
       <c r="M4">
-        <v>8</v>
-      </c>
-      <c r="N4" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1246,13 +1581,13 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -1263,11 +1598,11 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="3">
-        <v>100</v>
+      <c r="I5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
@@ -1276,10 +1611,10 @@
         <v>20</v>
       </c>
       <c r="M5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1290,13 +1625,13 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -1320,10 +1655,7 @@
         <v>20</v>
       </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1334,13 +1666,13 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -1351,11 +1683,11 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>22</v>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="3">
+        <v>100</v>
       </c>
       <c r="K7" t="s">
         <v>19</v>
@@ -1364,10 +1696,10 @@
         <v>20</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1378,13 +1710,13 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -1408,10 +1740,10 @@
         <v>20</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1422,13 +1754,13 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -1452,10 +1784,10 @@
         <v>20</v>
       </c>
       <c r="M9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1466,13 +1798,13 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1483,11 +1815,11 @@
       <c r="H10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="3">
-        <v>100</v>
+      <c r="I10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K10" t="s">
         <v>19</v>
@@ -1496,13 +1828,13 @@
         <v>20</v>
       </c>
       <c r="M10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1510,13 +1842,13 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -1528,10 +1860,10 @@
         <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="J11" s="3">
+        <v>100</v>
       </c>
       <c r="K11" t="s">
         <v>19</v>
@@ -1540,13 +1872,298 @@
         <v>20</v>
       </c>
       <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="3">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14">
         <v>5</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N14" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18">
+        <v>1001</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1556,7 +2173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327BB445-E756-4647-886B-5441E232C968}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#Added Code for SYDATAT transaction RSTK-9118,RSTK-9119,RSTK-9120,RSTK-9121,RSTK-9122
#Added new Test Plan:API-InventoryTransactions in build.xml

#Modified .testProject file to make compatible for Parallel Execution
</commit_message>
<xml_diff>
--- a/templates/Division To division Transfer.xlsx
+++ b/templates/Division To division Transfer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0D7573-2459-4D4F-BF8A-68E8791368C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65308C33-CFA1-446F-A79E-5ED28A2F7B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BB441E9F-4FBE-410A-8F63-C9ADD7579EED}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,16 +703,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -723,8 +720,8 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
-        <v>36</v>
+      <c r="I2" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -733,10 +730,7 @@
         <v>21</v>
       </c>
       <c r="L2">
-        <v>100</v>
-      </c>
-      <c r="M2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -761,8 +755,8 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>53</v>
+      <c r="I3" t="s">
+        <v>36</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -771,7 +765,7 @@
         <v>21</v>
       </c>
       <c r="L3">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -782,10 +776,10 @@
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -796,8 +790,8 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
-        <v>36</v>
+      <c r="I4" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
@@ -806,7 +800,7 @@
         <v>21</v>
       </c>
       <c r="L4">
-        <v>75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -820,10 +814,10 @@
         <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+        <v>66</v>
+      </c>
+      <c r="F5">
+        <v>1001</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -831,8 +825,8 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>53</v>
+      <c r="I5" t="s">
+        <v>36</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
@@ -841,7 +835,7 @@
         <v>21</v>
       </c>
       <c r="L5">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -851,14 +845,14 @@
       <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>49</v>
+      <c r="C6" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6">
-        <v>1001</v>
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -866,8 +860,8 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
-        <v>36</v>
+      <c r="I6" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J6" t="s">
         <v>19</v>
@@ -876,7 +870,7 @@
         <v>21</v>
       </c>
       <c r="L6">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -901,8 +895,8 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>53</v>
+      <c r="I7" t="s">
+        <v>36</v>
       </c>
       <c r="J7" t="s">
         <v>19</v>
@@ -911,7 +905,7 @@
         <v>21</v>
       </c>
       <c r="L7">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -922,10 +916,10 @@
         <v>60</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -937,7 +931,7 @@
         <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
         <v>19</v>
@@ -946,7 +940,7 @@
         <v>21</v>
       </c>
       <c r="L8">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -956,11 +950,11 @@
       <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -972,7 +966,7 @@
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -981,21 +975,21 @@
         <v>21</v>
       </c>
       <c r="L9">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
+      <c r="A10" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>61</v>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1016,21 +1010,24 @@
         <v>21</v>
       </c>
       <c r="L10">
-        <v>10</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>67</v>
+      <c r="A11" t="s">
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11">
-        <v>100</v>
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -1041,7 +1038,7 @@
       <c r="H11" t="s">
         <v>18</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="4" t="s">
         <v>53</v>
       </c>
       <c r="J11" t="s">
@@ -1051,7 +1048,10 @@
         <v>21</v>
       </c>
       <c r="L11">
-        <v>135</v>
+        <v>60</v>
+      </c>
+      <c r="M11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1079,8 +1079,8 @@
       <c r="H12" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>53</v>
+      <c r="I12" t="s">
+        <v>36</v>
       </c>
       <c r="J12" t="s">
         <v>19</v>
@@ -1089,10 +1089,10 @@
         <v>21</v>
       </c>
       <c r="L12">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="M12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1103,13 +1103,13 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1130,10 +1130,10 @@
         <v>21</v>
       </c>
       <c r="L13">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="M13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1144,13 +1144,13 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -1161,8 +1161,8 @@
       <c r="H14" t="s">
         <v>18</v>
       </c>
-      <c r="I14" t="s">
-        <v>36</v>
+      <c r="I14" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J14" t="s">
         <v>19</v>
@@ -1171,10 +1171,10 @@
         <v>21</v>
       </c>
       <c r="L14">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1202,8 +1202,8 @@
       <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>53</v>
+      <c r="I15" t="s">
+        <v>36</v>
       </c>
       <c r="J15" t="s">
         <v>19</v>
@@ -1212,10 +1212,10 @@
         <v>21</v>
       </c>
       <c r="L15">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="M15" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1226,13 +1226,13 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -1243,8 +1243,8 @@
       <c r="H16" t="s">
         <v>18</v>
       </c>
-      <c r="I16" t="s">
-        <v>36</v>
+      <c r="I16" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J16" t="s">
         <v>19</v>
@@ -1253,10 +1253,10 @@
         <v>21</v>
       </c>
       <c r="L16">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="M16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1267,13 +1267,13 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1284,7 +1284,7 @@
       <c r="H17" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" t="s">
         <v>53</v>
       </c>
       <c r="J17" t="s">
@@ -1294,10 +1294,10 @@
         <v>21</v>
       </c>
       <c r="L17">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="M17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1308,13 +1308,13 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
@@ -1326,7 +1326,7 @@
         <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
         <v>19</v>
@@ -1335,10 +1335,10 @@
         <v>21</v>
       </c>
       <c r="L18">
-        <v>10</v>
+        <v>135</v>
       </c>
       <c r="M18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1349,13 +1349,13 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
         <v>15</v>
@@ -1367,7 +1367,7 @@
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
@@ -1376,10 +1376,10 @@
         <v>21</v>
       </c>
       <c r="L19">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="M19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1466,11 +1466,11 @@
       <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>50</v>
+      <c r="C2" t="s">
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -1482,7 +1482,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
         <v>70</v>
@@ -1504,11 +1504,11 @@
       <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>51</v>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1520,7 +1520,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
         <v>70</v>
@@ -1532,18 +1532,18 @@
         <v>20</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>67</v>
+      <c r="A4" t="s">
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="C4">
-        <v>100</v>
+      <c r="C4" t="s">
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>65</v>
@@ -1558,7 +1558,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
         <v>70</v>
@@ -1570,7 +1570,7 @@
         <v>20</v>
       </c>
       <c r="M4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1578,19 +1578,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+        <v>66</v>
+      </c>
+      <c r="F5">
+        <v>1001</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -1599,10 +1596,10 @@
         <v>18</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>70</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
@@ -1611,10 +1608,7 @@
         <v>20</v>
       </c>
       <c r="M5">
-        <v>6</v>
-      </c>
-      <c r="N5" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1622,16 +1616,13 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -1643,10 +1634,10 @@
         <v>18</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>70</v>
       </c>
       <c r="K6" t="s">
         <v>19</v>
@@ -1655,7 +1646,7 @@
         <v>20</v>
       </c>
       <c r="M6">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1663,16 +1654,13 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -1683,11 +1671,11 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="3">
-        <v>100</v>
+      <c r="I7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>70</v>
       </c>
       <c r="K7" t="s">
         <v>19</v>
@@ -1696,27 +1684,21 @@
         <v>20</v>
       </c>
       <c r="M7">
-        <v>8</v>
-      </c>
-      <c r="N7" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
+      <c r="A8" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -1727,11 +1709,11 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="3">
-        <v>100</v>
+      <c r="I8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>70</v>
       </c>
       <c r="K8" t="s">
         <v>19</v>
@@ -1740,10 +1722,7 @@
         <v>20</v>
       </c>
       <c r="M8">
-        <v>7</v>
-      </c>
-      <c r="N8" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1754,13 +1733,13 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -1772,10 +1751,10 @@
         <v>18</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="K9" t="s">
         <v>19</v>
@@ -1784,10 +1763,10 @@
         <v>20</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1798,13 +1777,13 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1828,10 +1807,7 @@
         <v>20</v>
       </c>
       <c r="M10">
-        <v>6</v>
-      </c>
-      <c r="N10" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1842,13 +1818,13 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -1872,10 +1848,10 @@
         <v>20</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1886,13 +1862,13 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -1903,11 +1879,11 @@
       <c r="H12" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>22</v>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="3">
+        <v>100</v>
       </c>
       <c r="K12" t="s">
         <v>19</v>
@@ -1916,10 +1892,10 @@
         <v>20</v>
       </c>
       <c r="M12">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1930,13 +1906,13 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1947,11 +1923,11 @@
       <c r="H13" t="s">
         <v>18</v>
       </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="3">
-        <v>100</v>
+      <c r="I13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K13" t="s">
         <v>19</v>
@@ -1960,13 +1936,13 @@
         <v>20</v>
       </c>
       <c r="M13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1974,13 +1950,13 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -1991,11 +1967,11 @@
       <c r="H14" t="s">
         <v>18</v>
       </c>
-      <c r="I14" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>38</v>
+      <c r="I14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K14" t="s">
         <v>19</v>
@@ -2004,10 +1980,10 @@
         <v>20</v>
       </c>
       <c r="M14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -2015,13 +1991,16 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
@@ -2032,11 +2011,11 @@
       <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" t="s">
-        <v>70</v>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="3">
+        <v>100</v>
       </c>
       <c r="K15" t="s">
         <v>19</v>
@@ -2045,7 +2024,10 @@
         <v>20</v>
       </c>
       <c r="M15">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -2053,13 +2035,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -2071,10 +2056,10 @@
         <v>18</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" t="s">
-        <v>70</v>
+        <v>53</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K16" t="s">
         <v>19</v>
@@ -2083,21 +2068,27 @@
         <v>20</v>
       </c>
       <c r="M16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -2108,11 +2099,11 @@
       <c r="H17" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" t="s">
         <v>36</v>
       </c>
-      <c r="J17" t="s">
-        <v>70</v>
+      <c r="J17" s="3">
+        <v>100</v>
       </c>
       <c r="K17" t="s">
         <v>19</v>
@@ -2121,24 +2112,30 @@
         <v>20</v>
       </c>
       <c r="M17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="N17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18">
-        <v>1001</v>
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
       </c>
       <c r="G18" t="s">
         <v>17</v>
@@ -2146,11 +2143,11 @@
       <c r="H18" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" t="s">
-        <v>70</v>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="K18" t="s">
         <v>19</v>
@@ -2159,7 +2156,10 @@
         <v>20</v>
       </c>
       <c r="M18">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="N18" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>